<commit_message>
chore : documentation filled
</commit_message>
<xml_diff>
--- a/doc/Poktan.xlsx
+++ b/doc/Poktan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITERA\Kuliah Online\TA\Ackyras\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DD99A0-D344-452B-A67E-1A5DB82AD61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BF7C2D-5BDF-4E48-BE9D-EF955C327CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,21 @@
     <sheet name="Toba" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Toba!$A$1:$F$973</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Toba!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -7462,7 +7474,7 @@
   <dimension ref="A1:F973"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="89" zoomScaleNormal="100" zoomScaleSheetLayoutView="89" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C66" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
@@ -21678,10 +21690,13 @@
     <sortCondition ref="C2"/>
   </sortState>
   <pageMargins left="0.70866141732283472" right="0.31496062992125984" top="0.55118110236220474" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="5" scale="72" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="5" scale="65" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <rowBreaks count="2" manualBreakCount="2">
-    <brk id="213" max="6" man="1"/>
+    <brk id="213" max="5" man="1"/>
     <brk id="298" max="16383" man="1"/>
   </rowBreaks>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="6" max="1048575" man="1"/>
+  </colBreaks>
 </worksheet>
 </file>
</xml_diff>